<commit_message>
PAM data & code added
</commit_message>
<xml_diff>
--- a/data/GROWTH.xlsx
+++ b/data/GROWTH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anaislebrun/Desktop/These/Meso Tromso 2022/MHV_Tromso/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D6F54A-B768-6348-BB1A-1061226C44E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3424FB-1EB5-024D-A5AE-4DF4558BE5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,10 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -198,6 +195,13 @@
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -221,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -229,7 +233,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -453,7 +460,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -534,8 +541,7 @@
         <v>3.4</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H8" si="0">G2-2/23</f>
-        <v>3.3130434782608695</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>13</v>
@@ -568,8 +574,7 @@
         <v>3.1</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" si="0"/>
-        <v>3.0130434782608697</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>13</v>
@@ -602,8 +607,7 @@
         <v>3.5</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
-        <v>3.4130434782608696</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>13</v>
@@ -636,8 +640,7 @@
         <v>3</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="0"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>13</v>
@@ -670,8 +673,7 @@
         <v>5.5</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="0"/>
-        <v>5.4130434782608692</v>
+        <v>0.152</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>13</v>
@@ -704,8 +706,7 @@
         <v>2.4</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="0"/>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>13</v>
@@ -738,8 +739,7 @@
         <v>2.1</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="0"/>
-        <v>2.0130434782608697</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>13</v>
@@ -807,8 +807,7 @@
         <v>10</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" ref="H10:H55" si="1">G10-2/23</f>
-        <v>9.9130434782608692</v>
+        <v>0.34799999999999998</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>13</v>
@@ -841,8 +840,7 @@
         <v>2.9</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="1"/>
-        <v>2.8130434782608695</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>14</v>
@@ -875,8 +873,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="1"/>
-        <v>5.0130434782608688</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>14</v>
@@ -909,8 +906,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="1"/>
-        <v>9.7130434782608699</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>14</v>
@@ -943,8 +939,7 @@
         <v>9.9</v>
       </c>
       <c r="H14" s="3">
-        <f t="shared" si="1"/>
-        <v>9.8130434782608695</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>14</v>
@@ -977,8 +972,7 @@
         <v>3</v>
       </c>
       <c r="H15" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>13</v>
@@ -1011,8 +1005,7 @@
         <v>6</v>
       </c>
       <c r="H16" s="3">
-        <f t="shared" si="1"/>
-        <v>5.9130434782608692</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>13</v>
@@ -1045,8 +1038,7 @@
         <v>3.5</v>
       </c>
       <c r="H17" s="3">
-        <f t="shared" si="1"/>
-        <v>3.4130434782608696</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>13</v>
@@ -1079,8 +1071,7 @@
         <v>2.8</v>
       </c>
       <c r="H18" s="3">
-        <f t="shared" si="1"/>
-        <v>2.7130434782608694</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>13</v>
@@ -1113,8 +1104,7 @@
         <v>3</v>
       </c>
       <c r="H19" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>13</v>
@@ -1147,8 +1137,7 @@
         <v>4.7</v>
       </c>
       <c r="H20" s="3">
-        <f t="shared" si="1"/>
-        <v>4.6130434782608694</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>13</v>
@@ -1181,8 +1170,7 @@
         <v>5.7</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" si="1"/>
-        <v>5.6130434782608694</v>
+        <v>0.161</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>13</v>
@@ -1215,8 +1203,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" si="1"/>
-        <v>2.2130434782608694</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>13</v>
@@ -1249,8 +1236,7 @@
         <v>2</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" si="1"/>
-        <v>1.9130434782608696</v>
+        <v>0</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>14</v>
@@ -1283,8 +1269,7 @@
         <v>2</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="1"/>
-        <v>1.9130434782608696</v>
+        <v>0</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>14</v>
@@ -1317,8 +1302,7 @@
         <v>7.1</v>
       </c>
       <c r="H25" s="3">
-        <f t="shared" si="1"/>
-        <v>7.0130434782608688</v>
+        <v>0.222</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>14</v>
@@ -1351,8 +1335,7 @@
         <v>7.4</v>
       </c>
       <c r="H26" s="3">
-        <f t="shared" si="1"/>
-        <v>7.3130434782608695</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>14</v>
@@ -1385,8 +1368,7 @@
         <v>2.8</v>
       </c>
       <c r="H27" s="3">
-        <f t="shared" si="1"/>
-        <v>2.7130434782608694</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>14</v>
@@ -1419,8 +1401,7 @@
         <v>2.6</v>
       </c>
       <c r="H28" s="3">
-        <f t="shared" si="1"/>
-        <v>2.5130434782608697</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>14</v>
@@ -1453,8 +1434,7 @@
         <v>3</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>13</v>
@@ -1487,8 +1467,7 @@
         <v>2.5</v>
       </c>
       <c r="H30" s="3">
-        <f t="shared" si="1"/>
-        <v>2.4130434782608696</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>13</v>
@@ -1521,8 +1500,7 @@
         <v>2.5</v>
       </c>
       <c r="H31" s="3">
-        <f t="shared" si="1"/>
-        <v>2.4130434782608696</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>13</v>
@@ -1555,8 +1533,7 @@
         <v>2.8</v>
       </c>
       <c r="H32" s="3">
-        <f t="shared" si="1"/>
-        <v>2.7130434782608694</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>13</v>
@@ -1589,8 +1566,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="3">
-        <f t="shared" si="1"/>
-        <v>4.9130434782608692</v>
+        <v>0.13</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>13</v>
@@ -1625,8 +1601,7 @@
         <v>2.4</v>
       </c>
       <c r="H34" s="3">
-        <f t="shared" si="1"/>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>14</v>
@@ -1659,8 +1634,7 @@
         <v>3.4</v>
       </c>
       <c r="H35" s="3">
-        <f t="shared" si="1"/>
-        <v>3.3130434782608695</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>14</v>
@@ -1693,8 +1667,7 @@
         <v>7.5</v>
       </c>
       <c r="H36" s="3">
-        <f t="shared" si="1"/>
-        <v>7.4130434782608692</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>14</v>
@@ -1729,8 +1702,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="H37" s="3">
-        <f t="shared" si="1"/>
-        <v>8.6130434782608685</v>
+        <v>0.29099999999999998</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>14</v>
@@ -1763,8 +1735,7 @@
         <v>2.1</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0130434782608697</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>14</v>
@@ -1797,8 +1768,7 @@
         <v>2.1</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" si="1"/>
-        <v>2.0130434782608697</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>14</v>
@@ -1831,8 +1801,7 @@
         <v>3.3</v>
       </c>
       <c r="H40" s="3">
-        <f t="shared" si="1"/>
-        <v>3.2130434782608694</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>13</v>
@@ -1865,8 +1834,7 @@
         <v>3</v>
       </c>
       <c r="H41" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>13</v>
@@ -1899,8 +1867,7 @@
         <v>2.5</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="1"/>
-        <v>2.4130434782608696</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>13</v>
@@ -1933,8 +1900,7 @@
         <v>4</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" si="1"/>
-        <v>3.9130434782608696</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>13</v>
@@ -1967,8 +1933,7 @@
         <v>3</v>
       </c>
       <c r="H44" s="3">
-        <f t="shared" si="1"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>13</v>
@@ -2001,8 +1966,7 @@
         <v>8</v>
       </c>
       <c r="H45" s="3">
-        <f t="shared" si="1"/>
-        <v>7.9130434782608692</v>
+        <v>0.26100000000000001</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>13</v>
@@ -2035,8 +1999,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="H46" s="3">
-        <f t="shared" si="1"/>
-        <v>8.1130434782608685</v>
+        <v>0.27</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>13</v>
@@ -2069,8 +2032,7 @@
         <v>3.5</v>
       </c>
       <c r="H47" s="3">
-        <f t="shared" si="1"/>
-        <v>3.4130434782608696</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>14</v>
@@ -2103,8 +2065,7 @@
         <v>2.9</v>
       </c>
       <c r="H48" s="3">
-        <f t="shared" si="1"/>
-        <v>2.8130434782608695</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>14</v>
@@ -2137,8 +2098,7 @@
         <v>5.9</v>
       </c>
       <c r="H49" s="3">
-        <f t="shared" si="1"/>
-        <v>5.8130434782608695</v>
+        <v>0.17</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>14</v>
@@ -2173,8 +2133,7 @@
         <v>7.4</v>
       </c>
       <c r="H50" s="3">
-        <f t="shared" si="1"/>
-        <v>7.3130434782608695</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>14</v>
@@ -2207,8 +2166,7 @@
         <v>2.4</v>
       </c>
       <c r="H51" s="3">
-        <f t="shared" si="1"/>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>14</v>
@@ -2241,8 +2199,7 @@
         <v>2.5</v>
       </c>
       <c r="H52" s="3">
-        <f t="shared" si="1"/>
-        <v>2.4130434782608696</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>14</v>
@@ -2275,8 +2232,7 @@
         <v>2.5</v>
       </c>
       <c r="H53" s="3">
-        <f t="shared" si="1"/>
-        <v>2.4130434782608696</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>13</v>
@@ -2309,8 +2265,7 @@
         <v>4.8</v>
       </c>
       <c r="H54" s="3">
-        <f t="shared" si="1"/>
-        <v>4.713043478260869</v>
+        <v>0.122</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>13</v>
@@ -2343,8 +2298,7 @@
         <v>2.8</v>
       </c>
       <c r="H55" s="3">
-        <f t="shared" si="1"/>
-        <v>2.7130434782608694</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>13</v>
@@ -2410,8 +2364,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="H57" s="3">
-        <f>G57-2/23</f>
-        <v>8.2130434782608699</v>
+        <v>0.27400000000000002</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>13</v>
@@ -2477,8 +2430,7 @@
         <v>2.6</v>
       </c>
       <c r="H59" s="3">
-        <f t="shared" ref="H59:H61" si="2">G59-2/23</f>
-        <v>2.5130434782608697</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>14</v>
@@ -2511,8 +2463,7 @@
         <v>2.8</v>
       </c>
       <c r="H60" s="3">
-        <f t="shared" si="2"/>
-        <v>2.7130434782608694</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>14</v>
@@ -2545,8 +2496,7 @@
         <v>7.3</v>
       </c>
       <c r="H61" s="3">
-        <f t="shared" si="2"/>
-        <v>7.213043478260869</v>
+        <v>0.23</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>14</v>
@@ -2614,8 +2564,7 @@
         <v>2.6</v>
       </c>
       <c r="H63" s="3">
-        <f t="shared" ref="H63:H74" si="3">G63-2/23</f>
-        <v>2.5130434782608697</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>14</v>
@@ -2648,8 +2597,7 @@
         <v>2.9</v>
       </c>
       <c r="H64" s="3">
-        <f t="shared" si="3"/>
-        <v>2.8130434782608695</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>14</v>
@@ -2682,8 +2630,7 @@
         <v>5</v>
       </c>
       <c r="H65" s="3">
-        <f t="shared" si="3"/>
-        <v>4.9130434782608692</v>
+        <v>0.13</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>13</v>
@@ -2716,8 +2663,7 @@
         <v>2.4</v>
       </c>
       <c r="H66" s="3">
-        <f t="shared" si="3"/>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>13</v>
@@ -2750,8 +2696,7 @@
         <v>2</v>
       </c>
       <c r="H67" s="3">
-        <f t="shared" si="3"/>
-        <v>1.9130434782608696</v>
+        <v>0</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>13</v>
@@ -2784,8 +2729,7 @@
         <v>3.8</v>
       </c>
       <c r="H68" s="3">
-        <f t="shared" si="3"/>
-        <v>3.7130434782608694</v>
+        <v>7.8E-2</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>13</v>
@@ -2818,8 +2762,7 @@
         <v>4.5</v>
       </c>
       <c r="H69" s="3">
-        <f t="shared" si="3"/>
-        <v>4.4130434782608692</v>
+        <v>0.109</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>13</v>
@@ -2852,8 +2795,7 @@
         <v>9</v>
       </c>
       <c r="H70" s="3">
-        <f t="shared" si="3"/>
-        <v>8.9130434782608692</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>13</v>
@@ -2886,8 +2828,7 @@
         <v>3.1</v>
       </c>
       <c r="H71" s="3">
-        <f t="shared" si="3"/>
-        <v>3.0130434782608697</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>14</v>
@@ -2920,8 +2861,7 @@
         <v>3.4</v>
       </c>
       <c r="H72" s="3">
-        <f t="shared" si="3"/>
-        <v>3.3130434782608695</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>14</v>
@@ -2954,8 +2894,7 @@
         <v>9.8000000000000007</v>
       </c>
       <c r="H73" s="3">
-        <f t="shared" si="3"/>
-        <v>9.7130434782608699</v>
+        <v>0.33900000000000002</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>14</v>
@@ -2988,8 +2927,7 @@
         <v>5.9</v>
       </c>
       <c r="H74" s="3">
-        <f t="shared" si="3"/>
-        <v>5.8130434782608695</v>
+        <v>0.17</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>14</v>
@@ -3055,8 +2993,7 @@
         <v>2.1</v>
       </c>
       <c r="H76" s="3">
-        <f t="shared" ref="H76:H91" si="4">G76-2/23</f>
-        <v>2.0130434782608697</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I76" s="2" t="s">
         <v>14</v>
@@ -3089,8 +3026,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H77" s="3">
-        <f t="shared" si="4"/>
-        <v>2.2130434782608694</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I77" s="2" t="s">
         <v>13</v>
@@ -3123,8 +3059,7 @@
         <v>5</v>
       </c>
       <c r="H78" s="3">
-        <f t="shared" si="4"/>
-        <v>4.9130434782608692</v>
+        <v>0.13</v>
       </c>
       <c r="I78" s="2" t="s">
         <v>13</v>
@@ -3157,8 +3092,7 @@
         <v>7.5</v>
       </c>
       <c r="H79" s="3">
-        <f t="shared" si="4"/>
-        <v>7.4130434782608692</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>13</v>
@@ -3191,8 +3125,7 @@
         <v>3</v>
       </c>
       <c r="H80" s="3">
-        <f t="shared" si="4"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I80" s="2" t="s">
         <v>13</v>
@@ -3225,8 +3158,7 @@
         <v>4.2</v>
       </c>
       <c r="H81" s="3">
-        <f t="shared" si="4"/>
-        <v>4.1130434782608694</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="I81" s="2" t="s">
         <v>13</v>
@@ -3259,8 +3191,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H82" s="3">
-        <f t="shared" si="4"/>
-        <v>2.1130434782608698</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I82" s="2" t="s">
         <v>13</v>
@@ -3293,8 +3224,7 @@
         <v>4.5</v>
       </c>
       <c r="H83" s="3">
-        <f t="shared" si="4"/>
-        <v>4.4130434782608692</v>
+        <v>0.109</v>
       </c>
       <c r="I83" s="2" t="s">
         <v>13</v>
@@ -3327,8 +3257,7 @@
         <v>6.7</v>
       </c>
       <c r="H84" s="3">
-        <f t="shared" si="4"/>
-        <v>6.6130434782608694</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="I84" s="2" t="s">
         <v>13</v>
@@ -3361,8 +3290,7 @@
         <v>9.5</v>
       </c>
       <c r="H85" s="3">
-        <f t="shared" si="4"/>
-        <v>9.4130434782608692</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="I85" s="2" t="s">
         <v>13</v>
@@ -3395,8 +3323,7 @@
         <v>2.8</v>
       </c>
       <c r="H86" s="3">
-        <f t="shared" si="4"/>
-        <v>2.7130434782608694</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I86" s="2" t="s">
         <v>14</v>
@@ -3429,8 +3356,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="H87" s="3">
-        <f t="shared" si="4"/>
-        <v>4.0130434782608688</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="I87" s="2" t="s">
         <v>14</v>
@@ -3463,8 +3389,7 @@
         <v>10.9</v>
       </c>
       <c r="H88" s="3">
-        <f t="shared" si="4"/>
-        <v>10.81304347826087</v>
+        <v>0.38700000000000001</v>
       </c>
       <c r="I88" s="2" t="s">
         <v>14</v>
@@ -3497,8 +3422,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="H89" s="3">
-        <f t="shared" si="4"/>
-        <v>9.2130434782608699</v>
+        <v>0.317</v>
       </c>
       <c r="I89" s="2" t="s">
         <v>14</v>
@@ -3531,8 +3455,7 @@
         <v>2.7</v>
       </c>
       <c r="H90" s="3">
-        <f t="shared" si="4"/>
-        <v>2.6130434782608698</v>
+        <v>0.03</v>
       </c>
       <c r="I90" s="2" t="s">
         <v>14</v>
@@ -3565,8 +3488,7 @@
         <v>2.9</v>
       </c>
       <c r="H91" s="3">
-        <f t="shared" si="4"/>
-        <v>2.8130434782608695</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I91" s="2" t="s">
         <v>14</v>
@@ -3669,8 +3591,7 @@
         <v>3.5</v>
       </c>
       <c r="H94" s="3">
-        <f t="shared" ref="H94:H102" si="5">G94-2/23</f>
-        <v>3.4130434782608696</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="I94" s="2" t="s">
         <v>13</v>
@@ -3703,8 +3624,7 @@
         <v>3.6</v>
       </c>
       <c r="H95" s="3">
-        <f t="shared" si="5"/>
-        <v>3.5130434782608697</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I95" s="2" t="s">
         <v>13</v>
@@ -3737,8 +3657,7 @@
         <v>3.5</v>
       </c>
       <c r="H96" s="3">
-        <f t="shared" si="5"/>
-        <v>3.4130434782608696</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="I96" s="2" t="s">
         <v>13</v>
@@ -3771,8 +3690,7 @@
         <v>5</v>
       </c>
       <c r="H97" s="3">
-        <f t="shared" si="5"/>
-        <v>4.9130434782608692</v>
+        <v>0.13</v>
       </c>
       <c r="I97" s="2" t="s">
         <v>13</v>
@@ -3805,8 +3723,7 @@
         <v>2.5</v>
       </c>
       <c r="H98" s="3">
-        <f t="shared" si="5"/>
-        <v>2.4130434782608696</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I98" s="2" t="s">
         <v>13</v>
@@ -3839,8 +3756,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H99" s="3">
-        <f t="shared" si="5"/>
-        <v>2.1130434782608698</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>13</v>
@@ -3873,8 +3789,7 @@
         <v>3.9</v>
       </c>
       <c r="H100" s="3">
-        <f t="shared" si="5"/>
-        <v>3.8130434782608695</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>14</v>
@@ -3907,8 +3822,7 @@
         <v>5.2</v>
       </c>
       <c r="H101" s="3">
-        <f t="shared" si="5"/>
-        <v>5.1130434782608694</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="I101" s="2" t="s">
         <v>14</v>
@@ -3941,8 +3855,7 @@
         <v>7.1</v>
       </c>
       <c r="H102" s="3">
-        <f t="shared" si="5"/>
-        <v>7.0130434782608688</v>
+        <v>0.222</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>14</v>
@@ -4012,8 +3925,7 @@
         <v>2.6</v>
       </c>
       <c r="H104" s="3">
-        <f t="shared" ref="H104:H111" si="6">G104-2/23</f>
-        <v>2.5130434782608697</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>14</v>
@@ -4046,8 +3958,7 @@
         <v>2.8</v>
       </c>
       <c r="H105" s="3">
-        <f t="shared" si="6"/>
-        <v>2.7130434782608694</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>14</v>
@@ -4080,8 +3991,7 @@
         <v>2.4</v>
       </c>
       <c r="H106" s="3">
-        <f t="shared" si="6"/>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>13</v>
@@ -4114,8 +4024,7 @@
         <v>2.9</v>
       </c>
       <c r="H107" s="3">
-        <f t="shared" si="6"/>
-        <v>2.8130434782608695</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I107" s="2" t="s">
         <v>13</v>
@@ -4150,8 +4059,7 @@
         <v>3</v>
       </c>
       <c r="H108" s="3">
-        <f t="shared" si="6"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>13</v>
@@ -4184,8 +4092,7 @@
         <v>3.1</v>
       </c>
       <c r="H109" s="3">
-        <f t="shared" si="6"/>
-        <v>3.0130434782608697</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="I109" s="2" t="s">
         <v>13</v>
@@ -4218,8 +4125,7 @@
         <v>6.6</v>
       </c>
       <c r="H110" s="3">
-        <f t="shared" si="6"/>
-        <v>6.5130434782608688</v>
+        <v>0.2</v>
       </c>
       <c r="I110" s="2" t="s">
         <v>13</v>
@@ -4252,8 +4158,7 @@
         <v>3.2</v>
       </c>
       <c r="H111" s="3">
-        <f t="shared" si="6"/>
-        <v>3.1130434782608698</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="I111" s="2" t="s">
         <v>13</v>
@@ -4321,8 +4226,7 @@
         <v>3.7</v>
       </c>
       <c r="H113" s="3">
-        <f t="shared" ref="H113:H130" si="7">G113-2/23</f>
-        <v>3.6130434782608698</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="I113" s="2" t="s">
         <v>14</v>
@@ -4355,8 +4259,7 @@
         <v>4.8</v>
       </c>
       <c r="H114" s="3">
-        <f t="shared" si="7"/>
-        <v>4.713043478260869</v>
+        <v>0.122</v>
       </c>
       <c r="I114" s="2" t="s">
         <v>14</v>
@@ -4389,8 +4292,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="H115" s="3">
-        <f t="shared" si="7"/>
-        <v>9.2130434782608699</v>
+        <v>0.317</v>
       </c>
       <c r="I115" s="2" t="s">
         <v>14</v>
@@ -4423,8 +4325,7 @@
         <v>7.1</v>
       </c>
       <c r="H116" s="3">
-        <f t="shared" si="7"/>
-        <v>7.0130434782608688</v>
+        <v>0.222</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>14</v>
@@ -4457,8 +4358,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="H117" s="3">
-        <f t="shared" si="7"/>
-        <v>2.2130434782608694</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>14</v>
@@ -4491,8 +4391,7 @@
         <v>2.4</v>
       </c>
       <c r="H118" s="3">
-        <f t="shared" si="7"/>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>14</v>
@@ -4525,8 +4424,7 @@
         <v>6</v>
       </c>
       <c r="H119" s="3">
-        <f t="shared" si="7"/>
-        <v>5.9130434782608692</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>13</v>
@@ -4559,8 +4457,7 @@
         <v>3.3</v>
       </c>
       <c r="H120" s="3">
-        <f t="shared" si="7"/>
-        <v>3.2130434782608694</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>13</v>
@@ -4593,8 +4490,7 @@
         <v>3.8</v>
       </c>
       <c r="H121" s="3">
-        <f t="shared" si="7"/>
-        <v>3.7130434782608694</v>
+        <v>7.8E-2</v>
       </c>
       <c r="I121" s="2" t="s">
         <v>13</v>
@@ -4627,8 +4523,7 @@
         <v>4</v>
       </c>
       <c r="H122" s="3">
-        <f t="shared" si="7"/>
-        <v>3.9130434782608696</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="I122" s="2" t="s">
         <v>13</v>
@@ -4661,8 +4556,7 @@
         <v>3</v>
       </c>
       <c r="H123" s="3">
-        <f t="shared" si="7"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I123" s="2" t="s">
         <v>13</v>
@@ -4695,8 +4589,7 @@
         <v>3</v>
       </c>
       <c r="H124" s="3">
-        <f t="shared" si="7"/>
-        <v>2.9130434782608696</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="I124" s="2" t="s">
         <v>13</v>
@@ -4729,8 +4622,7 @@
         <v>2.5</v>
       </c>
       <c r="H125" s="3">
-        <f t="shared" si="7"/>
-        <v>2.4130434782608696</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I125" s="2" t="s">
         <v>13</v>
@@ -4763,8 +4655,7 @@
         <v>2.7</v>
       </c>
       <c r="H126" s="3">
-        <f t="shared" si="7"/>
-        <v>2.6130434782608698</v>
+        <v>0.03</v>
       </c>
       <c r="I126" s="2" t="s">
         <v>13</v>
@@ -4797,8 +4688,7 @@
         <v>5.3</v>
       </c>
       <c r="H127" s="3">
-        <f t="shared" si="7"/>
-        <v>5.213043478260869</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="I127" s="2" t="s">
         <v>14</v>
@@ -4831,8 +4721,7 @@
         <v>2.9</v>
       </c>
       <c r="H128" s="3">
-        <f t="shared" si="7"/>
-        <v>2.8130434782608695</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I128" s="2" t="s">
         <v>14</v>
@@ -4865,8 +4754,7 @@
         <v>5.2</v>
       </c>
       <c r="H129" s="3">
-        <f t="shared" si="7"/>
-        <v>5.1130434782608694</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="I129" s="2" t="s">
         <v>14</v>
@@ -4899,8 +4787,7 @@
         <v>6.2</v>
       </c>
       <c r="H130" s="3">
-        <f t="shared" si="7"/>
-        <v>6.1130434782608694</v>
+        <v>0.183</v>
       </c>
       <c r="I130" s="2" t="s">
         <v>14</v>
@@ -4966,8 +4853,7 @@
         <v>2.4</v>
       </c>
       <c r="H132" s="3">
-        <f t="shared" ref="H132:H137" si="8">G132-2/23</f>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I132" s="2" t="s">
         <v>14</v>
@@ -5000,8 +4886,7 @@
         <v>4.7</v>
       </c>
       <c r="H133" s="3">
-        <f t="shared" si="8"/>
-        <v>4.6130434782608694</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="I133" s="2" t="s">
         <v>13</v>
@@ -5034,8 +4919,7 @@
         <v>3.1</v>
       </c>
       <c r="H134" s="3">
-        <f t="shared" si="8"/>
-        <v>3.0130434782608697</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="I134" s="2" t="s">
         <v>13</v>
@@ -5068,8 +4952,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="H135" s="3">
-        <f t="shared" si="8"/>
-        <v>2.1130434782608698</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="I135" s="2" t="s">
         <v>13</v>
@@ -5102,8 +4985,7 @@
         <v>3.8</v>
       </c>
       <c r="H136" s="3">
-        <f t="shared" si="8"/>
-        <v>3.7130434782608694</v>
+        <v>7.8E-2</v>
       </c>
       <c r="I136" s="2" t="s">
         <v>13</v>
@@ -5136,8 +5018,7 @@
         <v>2.1</v>
       </c>
       <c r="H137" s="3">
-        <f t="shared" si="8"/>
-        <v>2.0130434782608697</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I137" s="2" t="s">
         <v>13</v>
@@ -5205,8 +5086,7 @@
         <v>10.5</v>
       </c>
       <c r="H139" s="3">
-        <f t="shared" ref="H139:H155" si="9">G139-2/23</f>
-        <v>10.413043478260869</v>
+        <v>0.37</v>
       </c>
       <c r="I139" s="2" t="s">
         <v>14</v>
@@ -5239,8 +5119,7 @@
         <v>7.6</v>
       </c>
       <c r="H140" s="3">
-        <f t="shared" si="9"/>
-        <v>7.5130434782608688</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="I140" s="2" t="s">
         <v>14</v>
@@ -5273,8 +5152,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H141" s="3">
-        <f t="shared" si="9"/>
-        <v>4.3130434782608695</v>
+        <v>0.104</v>
       </c>
       <c r="I141" s="2" t="s">
         <v>14</v>
@@ -5307,8 +5185,7 @@
         <v>3.3</v>
       </c>
       <c r="H142" s="3">
-        <f t="shared" si="9"/>
-        <v>3.2130434782608694</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="I142" s="2" t="s">
         <v>14</v>
@@ -5341,8 +5218,7 @@
         <v>6.6</v>
       </c>
       <c r="H143" s="3">
-        <f t="shared" si="9"/>
-        <v>6.5130434782608688</v>
+        <v>0.2</v>
       </c>
       <c r="I143" s="2" t="s">
         <v>14</v>
@@ -5375,8 +5251,7 @@
         <v>6.7</v>
       </c>
       <c r="H144" s="3">
-        <f t="shared" si="9"/>
-        <v>6.6130434782608694</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="I144" s="2" t="s">
         <v>14</v>
@@ -5409,8 +5284,7 @@
         <v>2.1</v>
       </c>
       <c r="H145" s="3">
-        <f t="shared" si="9"/>
-        <v>2.0130434782608697</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="I145" s="2" t="s">
         <v>14</v>
@@ -5443,8 +5317,7 @@
         <v>2.4</v>
       </c>
       <c r="H146" s="3">
-        <f t="shared" si="9"/>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I146" s="2" t="s">
         <v>14</v>
@@ -5477,8 +5350,7 @@
         <v>3.6</v>
       </c>
       <c r="H147" s="3">
-        <f t="shared" si="9"/>
-        <v>3.5130434782608697</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="I147" s="2" t="s">
         <v>13</v>
@@ -5511,8 +5383,7 @@
         <v>3.2</v>
       </c>
       <c r="H148" s="3">
-        <f t="shared" si="9"/>
-        <v>3.1130434782608698</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="I148" s="2" t="s">
         <v>13</v>
@@ -5545,8 +5416,7 @@
         <v>2.8</v>
       </c>
       <c r="H149" s="3">
-        <f t="shared" si="9"/>
-        <v>2.7130434782608694</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="I149" s="2" t="s">
         <v>13</v>
@@ -5579,8 +5449,7 @@
         <v>2.6</v>
       </c>
       <c r="H150" s="3">
-        <f t="shared" si="9"/>
-        <v>2.5130434782608697</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I150" s="2" t="s">
         <v>13</v>
@@ -5613,8 +5482,7 @@
         <v>2.5</v>
       </c>
       <c r="H151" s="3">
-        <f t="shared" si="9"/>
-        <v>2.4130434782608696</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="I151" s="2" t="s">
         <v>13</v>
@@ -5647,8 +5515,7 @@
         <v>2.9</v>
       </c>
       <c r="H152" s="3">
-        <f t="shared" si="9"/>
-        <v>2.8130434782608695</v>
+        <v>3.9E-2</v>
       </c>
       <c r="I152" s="2" t="s">
         <v>13</v>
@@ -5681,8 +5548,7 @@
         <v>2.4</v>
       </c>
       <c r="H153" s="3">
-        <f t="shared" si="9"/>
-        <v>2.3130434782608695</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="I153" s="2" t="s">
         <v>13</v>
@@ -5715,8 +5581,7 @@
         <v>6.2</v>
       </c>
       <c r="H154" s="3">
-        <f t="shared" si="9"/>
-        <v>6.1130434782608694</v>
+        <v>0.183</v>
       </c>
       <c r="I154" s="2" t="s">
         <v>13</v>
@@ -5749,8 +5614,7 @@
         <v>6.5</v>
       </c>
       <c r="H155" s="3">
-        <f t="shared" si="9"/>
-        <v>6.4130434782608692</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="I155" s="2" t="s">
         <v>13</v>
@@ -5816,8 +5680,7 @@
         <v>9</v>
       </c>
       <c r="H157" s="3">
-        <f t="shared" ref="H157:H163" si="10">G157-2/23</f>
-        <v>8.9130434782608692</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="I157" s="2" t="s">
         <v>14</v>
@@ -5850,8 +5713,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="H158" s="3">
-        <f t="shared" si="10"/>
-        <v>4.8130434782608695</v>
+        <v>0.126</v>
       </c>
       <c r="I158" s="2" t="s">
         <v>14</v>
@@ -5884,8 +5746,7 @@
         <v>4.5</v>
       </c>
       <c r="H159" s="3">
-        <f t="shared" si="10"/>
-        <v>4.4130434782608692</v>
+        <v>0.109</v>
       </c>
       <c r="I159" s="2" t="s">
         <v>14</v>
@@ -5918,8 +5779,7 @@
         <v>6.9</v>
       </c>
       <c r="H160" s="3">
-        <f t="shared" si="10"/>
-        <v>6.8130434782608695</v>
+        <v>0.21299999999999999</v>
       </c>
       <c r="I160" s="2" t="s">
         <v>14</v>
@@ -5952,8 +5812,7 @@
         <v>12.5</v>
       </c>
       <c r="H161" s="3">
-        <f t="shared" si="10"/>
-        <v>12.413043478260869</v>
+        <v>0.45700000000000002</v>
       </c>
       <c r="I161" s="2" t="s">
         <v>14</v>
@@ -5986,8 +5845,7 @@
         <v>2.6</v>
       </c>
       <c r="H162" s="3">
-        <f t="shared" si="10"/>
-        <v>2.5130434782608697</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="I162" s="2" t="s">
         <v>14</v>
@@ -6020,8 +5878,7 @@
         <v>2.7</v>
       </c>
       <c r="H163" s="3">
-        <f t="shared" si="10"/>
-        <v>2.6130434782608698</v>
+        <v>0.03</v>
       </c>
       <c r="I163" s="2" t="s">
         <v>14</v>
@@ -16907,7 +16764,7 @@
       <c r="E1000" s="2"/>
       <c r="F1000" s="2"/>
       <c r="G1000" s="2"/>
-      <c r="H1000" s="3"/>
+      <c r="H1000" s="4"/>
       <c r="I1000" s="2"/>
       <c r="J1000" s="2"/>
       <c r="K1000" s="2"/>

</xml_diff>